<commit_message>
Deploying to gh-pages from  @ c7937a27435e8e474daa6a747bb6e8bc212c5148 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.xlsx
+++ b/en/downloads/data-excel/1.1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Working\ЦЕЛИ УСТОЙЧИВОГО РАЗВИТИЯ\ПОКАЗАТЕЛИ ЦУР 2020\Глобальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Глобальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -706,9 +706,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -727,7 +729,7 @@
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" customHeight="1">
+    <row r="1" spans="1:17" ht="30" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
@@ -748,7 +750,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="19.5" customHeight="1">
+    <row r="2" spans="1:17" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -769,7 +771,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="17.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:17" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -784,7 +786,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -833,8 +835,11 @@
       <c r="P4" s="14">
         <v>2019</v>
       </c>
+      <c r="Q4" s="14">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
@@ -883,8 +888,11 @@
       <c r="P5" s="7">
         <v>0</v>
       </c>
+      <c r="Q5" s="7">
+        <v>0.02</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
@@ -933,8 +941,11 @@
       <c r="P6" s="9">
         <v>0</v>
       </c>
+      <c r="Q6" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
@@ -983,8 +994,11 @@
       <c r="P7" s="9">
         <v>0</v>
       </c>
+      <c r="Q7" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -1033,8 +1047,11 @@
       <c r="P8" s="9">
         <v>0</v>
       </c>
+      <c r="Q8" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1083,8 +1100,11 @@
       <c r="P9" s="9">
         <v>0</v>
       </c>
+      <c r="Q9" s="9">
+        <v>0.54</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1">
+    <row r="10" spans="1:17" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
@@ -1133,8 +1153,11 @@
       <c r="P10" s="9">
         <v>0</v>
       </c>
+      <c r="Q10" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1">
+    <row r="11" spans="1:17" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
@@ -1183,8 +1206,11 @@
       <c r="P11" s="9">
         <v>0</v>
       </c>
+      <c r="Q11" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -1233,8 +1259,11 @@
       <c r="P12" s="9">
         <v>0</v>
       </c>
+      <c r="Q12" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" s="25" t="s">
         <v>26</v>
       </c>
@@ -1283,8 +1312,11 @@
       <c r="P13" s="9">
         <v>0</v>
       </c>
+      <c r="Q13" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="15.75" thickBot="1">
       <c r="A14" s="26" t="s">
         <v>28</v>
       </c>
@@ -1323,6 +1355,9 @@
       <c r="P14" s="10">
         <v>0</v>
       </c>
+      <c r="Q14" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ a596536d721dda7e09f8827e147eddd0c1cf4949 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.xlsx
+++ b/en/downloads/data-excel/1.1.1.xlsx
@@ -324,7 +324,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -405,6 +405,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -706,10 +712,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -729,7 +735,7 @@
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1">
+    <row r="1" spans="1:18" ht="30" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
@@ -750,7 +756,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="19.5" customHeight="1">
+    <row r="2" spans="1:18" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -771,7 +777,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="17.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -786,7 +792,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -838,8 +844,11 @@
       <c r="Q4" s="14">
         <v>2020</v>
       </c>
+      <c r="R4" s="14">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
@@ -891,8 +900,11 @@
       <c r="Q5" s="7">
         <v>0.02</v>
       </c>
+      <c r="R5" s="29">
+        <v>8.0841202038693286E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
@@ -944,8 +956,11 @@
       <c r="Q6" s="9">
         <v>0</v>
       </c>
+      <c r="R6" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
@@ -997,8 +1012,11 @@
       <c r="Q7" s="9">
         <v>0</v>
       </c>
+      <c r="R7" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -1050,8 +1068,11 @@
       <c r="Q8" s="9">
         <v>0</v>
       </c>
+      <c r="R8" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1103,8 +1124,11 @@
       <c r="Q9" s="9">
         <v>0.54</v>
       </c>
+      <c r="R9" s="30">
+        <v>0.2462269049859406</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1">
+    <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
@@ -1156,8 +1180,11 @@
       <c r="Q10" s="9">
         <v>0</v>
       </c>
+      <c r="R10" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
@@ -1209,8 +1236,11 @@
       <c r="Q11" s="9">
         <v>0</v>
       </c>
+      <c r="R11" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -1262,8 +1292,11 @@
       <c r="Q12" s="9">
         <v>0</v>
       </c>
+      <c r="R12" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13" s="25" t="s">
         <v>26</v>
       </c>
@@ -1315,8 +1348,11 @@
       <c r="Q13" s="9">
         <v>0</v>
       </c>
+      <c r="R13" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1">
       <c r="A14" s="26" t="s">
         <v>28</v>
       </c>
@@ -1358,6 +1394,9 @@
       <c r="Q14" s="10">
         <v>0</v>
       </c>
+      <c r="R14" s="10">
+        <v>1.4177257229737372</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 0a351cd8e997bca2d3b51b362b3f1701cb4c3021 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.xlsx
+++ b/en/downloads/data-excel/1.1.1.xlsx
@@ -324,7 +324,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -405,12 +405,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -712,10 +706,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,7 +729,7 @@
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1">
+    <row r="1" spans="1:17" ht="30" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
@@ -756,7 +750,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="19.5" customHeight="1">
+    <row r="2" spans="1:17" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -777,7 +771,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:17" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -792,7 +786,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -844,11 +838,8 @@
       <c r="Q4" s="14">
         <v>2020</v>
       </c>
-      <c r="R4" s="14">
-        <v>2021</v>
-      </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
@@ -900,11 +891,8 @@
       <c r="Q5" s="7">
         <v>0.02</v>
       </c>
-      <c r="R5" s="29">
-        <v>8.0841202038693286E-2</v>
-      </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
@@ -956,11 +944,8 @@
       <c r="Q6" s="9">
         <v>0</v>
       </c>
-      <c r="R6" s="30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
@@ -1012,11 +997,8 @@
       <c r="Q7" s="9">
         <v>0</v>
       </c>
-      <c r="R7" s="30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -1068,11 +1050,8 @@
       <c r="Q8" s="9">
         <v>0</v>
       </c>
-      <c r="R8" s="30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1124,11 +1103,8 @@
       <c r="Q9" s="9">
         <v>0.54</v>
       </c>
-      <c r="R9" s="30">
-        <v>0.2462269049859406</v>
-      </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1">
+    <row r="10" spans="1:17" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
@@ -1180,11 +1156,8 @@
       <c r="Q10" s="9">
         <v>0</v>
       </c>
-      <c r="R10" s="30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1">
+    <row r="11" spans="1:17" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
@@ -1236,11 +1209,8 @@
       <c r="Q11" s="9">
         <v>0</v>
       </c>
-      <c r="R11" s="30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -1292,11 +1262,8 @@
       <c r="Q12" s="9">
         <v>0</v>
       </c>
-      <c r="R12" s="30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:17">
       <c r="A13" s="25" t="s">
         <v>26</v>
       </c>
@@ -1348,11 +1315,8 @@
       <c r="Q13" s="9">
         <v>0</v>
       </c>
-      <c r="R13" s="30">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="15.75" thickBot="1">
       <c r="A14" s="26" t="s">
         <v>28</v>
       </c>
@@ -1394,9 +1358,6 @@
       <c r="Q14" s="10">
         <v>0</v>
       </c>
-      <c r="R14" s="10">
-        <v>1.4177257229737372</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 205ef02c36b42275e832a02af2ccd64d053ef1fc 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.xlsx
+++ b/en/downloads/data-excel/1.1.1.xlsx
@@ -324,7 +324,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -405,6 +405,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -706,10 +712,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -729,7 +735,7 @@
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1">
+    <row r="1" spans="1:18" ht="30" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
@@ -750,7 +756,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="19.5" customHeight="1">
+    <row r="2" spans="1:18" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -771,7 +777,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="17.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -786,7 +792,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -838,8 +844,11 @@
       <c r="Q4" s="14">
         <v>2020</v>
       </c>
+      <c r="R4" s="14">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
@@ -891,8 +900,11 @@
       <c r="Q5" s="7">
         <v>0.02</v>
       </c>
+      <c r="R5" s="29">
+        <v>8.0841202038693286E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
@@ -944,8 +956,11 @@
       <c r="Q6" s="9">
         <v>0</v>
       </c>
+      <c r="R6" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
@@ -997,8 +1012,11 @@
       <c r="Q7" s="9">
         <v>0</v>
       </c>
+      <c r="R7" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -1050,8 +1068,11 @@
       <c r="Q8" s="9">
         <v>0</v>
       </c>
+      <c r="R8" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1103,8 +1124,11 @@
       <c r="Q9" s="9">
         <v>0.54</v>
       </c>
+      <c r="R9" s="30">
+        <v>0.2462269049859406</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1">
+    <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
@@ -1156,8 +1180,11 @@
       <c r="Q10" s="9">
         <v>0</v>
       </c>
+      <c r="R10" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
@@ -1209,8 +1236,11 @@
       <c r="Q11" s="9">
         <v>0</v>
       </c>
+      <c r="R11" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -1262,8 +1292,11 @@
       <c r="Q12" s="9">
         <v>0</v>
       </c>
+      <c r="R12" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13" s="25" t="s">
         <v>26</v>
       </c>
@@ -1315,8 +1348,11 @@
       <c r="Q13" s="9">
         <v>0</v>
       </c>
+      <c r="R13" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1">
       <c r="A14" s="26" t="s">
         <v>28</v>
       </c>
@@ -1358,6 +1394,9 @@
       <c r="Q14" s="10">
         <v>0</v>
       </c>
+      <c r="R14" s="10">
+        <v>1.4177257229737372</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ e324dde093680dfa498cd7aa82b8f416f5fc6d4f 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.xlsx
+++ b/en/downloads/data-excel/1.1.1.xlsx
@@ -712,10 +712,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,7 +735,7 @@
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1">
+    <row r="1" spans="1:19" ht="30" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="19.5" customHeight="1">
+    <row r="2" spans="1:19" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -777,7 +777,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:19" ht="17.25" customHeight="1" thickBot="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -792,7 +792,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
@@ -847,8 +847,11 @@
       <c r="R4" s="14">
         <v>2021</v>
       </c>
+      <c r="S4" s="14">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1">
+    <row r="5" spans="1:19" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
@@ -903,8 +906,11 @@
       <c r="R5" s="29">
         <v>8.0841202038693286E-2</v>
       </c>
+      <c r="S5" s="29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>14</v>
       </c>
@@ -959,8 +965,11 @@
       <c r="R6" s="30">
         <v>0</v>
       </c>
+      <c r="S6" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1">
+    <row r="7" spans="1:19" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
@@ -1015,8 +1024,11 @@
       <c r="R7" s="30">
         <v>0</v>
       </c>
+      <c r="S7" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1">
+    <row r="8" spans="1:19" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="s">
         <v>17</v>
       </c>
@@ -1071,8 +1083,11 @@
       <c r="R8" s="30">
         <v>0</v>
       </c>
+      <c r="S8" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1">
+    <row r="9" spans="1:19" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1127,8 +1142,11 @@
       <c r="R9" s="30">
         <v>0.2462269049859406</v>
       </c>
+      <c r="S9" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1">
+    <row r="10" spans="1:19" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
@@ -1183,8 +1201,11 @@
       <c r="R10" s="30">
         <v>0</v>
       </c>
+      <c r="S10" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1">
+    <row r="11" spans="1:19" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>22</v>
       </c>
@@ -1239,8 +1260,11 @@
       <c r="R11" s="30">
         <v>0</v>
       </c>
+      <c r="S11" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1">
+    <row r="12" spans="1:19" ht="15.75" customHeight="1">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -1295,8 +1319,11 @@
       <c r="R12" s="30">
         <v>0</v>
       </c>
+      <c r="S12" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" s="25" t="s">
         <v>26</v>
       </c>
@@ -1351,8 +1378,11 @@
       <c r="R13" s="30">
         <v>0</v>
       </c>
+      <c r="S13" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1">
+    <row r="14" spans="1:19" ht="15.75" thickBot="1">
       <c r="A14" s="26" t="s">
         <v>28</v>
       </c>
@@ -1397,6 +1427,9 @@
       <c r="R14" s="10">
         <v>1.4177257229737372</v>
       </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 29852311f9c5f8b61b2c29d7a4cfe07a70e22715 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.xlsx
+++ b/en/downloads/data-excel/1.1.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Кыргызская Республика</t>
   </si>
@@ -141,6 +141,85 @@
   </si>
   <si>
     <t>1.1.1 Proportion of population living below the international poverty line (1.9 USD)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <t>2022</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 2022-жылдан баштап, 2017-жылдагы САЖП боюнча бир адамга күнүнө 2,15 АКШ долларынан аз жашаган калктын үлүшү.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> С 2022 года, доля населения живущего менее чем на 2,15 долл. США на человека в день по ППС 2017 года.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> From 2022, the proportion of the population living on less than $2.15 per person per day in 2017 PPP.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -151,7 +230,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _р_._-;\-* #,##0.00\ _р_._-;_-* &quot;-&quot;??\ _р_._-;_-@_-"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +342,37 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -324,37 +434,17 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -406,11 +496,50 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -712,17 +841,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="1" max="3" width="35.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" customWidth="1"/>
@@ -735,231 +860,258 @@
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:20" ht="42" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
     </row>
-    <row r="2" spans="1:19" ht="19.5" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
     </row>
-    <row r="3" spans="1:19" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+    <row r="3" spans="1:20" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A3" s="24"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="5">
         <v>2007</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="5">
         <v>2008</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="5">
         <v>2009</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="5">
         <v>2010</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="5">
         <v>2011</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="6">
         <v>2012</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="6">
         <v>2013</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="6">
         <v>2014</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="5">
         <v>2015</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="6">
         <v>2016</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="6">
         <v>2017</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="6">
         <v>2018</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="6">
         <v>2019</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4" s="6">
         <v>2020</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="6">
         <v>2021</v>
       </c>
-      <c r="S4" s="14">
-        <v>2022</v>
+      <c r="S4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="6">
+        <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="25">
         <v>0.13164084338080392</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="25">
         <v>9.3408032246092107E-2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="25">
         <v>0.2920750078201626</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="25">
         <v>0.28004432896090853</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="25">
         <v>1.4718623476783729E-2</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="25">
         <v>0.28285601535166821</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="25">
         <v>0.33748893708707284</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="25">
         <v>7.0793627184116137E-2</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="26">
         <v>6.1812013361168511E-2</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="25">
         <v>0.20743278377239421</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="26">
         <v>0.31</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="26">
         <v>0.28000000000000003</v>
       </c>
-      <c r="P5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="7">
+      <c r="P5" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="26">
         <v>0.02</v>
       </c>
-      <c r="R5" s="29">
+      <c r="R5" s="27">
         <v>8.0841202038693286E-2</v>
       </c>
-      <c r="S5" s="29">
+      <c r="S5" s="27">
+        <v>0</v>
+      </c>
+      <c r="T5" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="D6" s="28">
+        <v>0</v>
+      </c>
+      <c r="E6" s="28">
         <v>0.27235776780828508</v>
       </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="F6" s="28">
+        <v>0</v>
+      </c>
+      <c r="G6" s="28">
         <v>0.2087126474406116</v>
       </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="9">
+      <c r="H6" s="28">
+        <v>0</v>
+      </c>
+      <c r="I6" s="28">
+        <v>0</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0</v>
+      </c>
+      <c r="K6" s="28">
+        <v>0</v>
+      </c>
+      <c r="L6" s="29">
         <v>0.33619680867967155</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="28">
         <v>0.32112435111554422</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="29">
         <v>1.08</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="29">
         <v>0.45</v>
       </c>
-      <c r="P6" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="9">
+      <c r="P6" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="29">
         <v>0</v>
       </c>
       <c r="R6" s="30">
@@ -968,57 +1120,60 @@
       <c r="S6" s="30">
         <v>0</v>
       </c>
+      <c r="T6" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="28">
         <v>0.20101785984326465</v>
       </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="E7" s="28">
+        <v>0</v>
+      </c>
+      <c r="F7" s="28">
+        <v>0</v>
+      </c>
+      <c r="G7" s="28">
         <v>0.21605756734684634</v>
       </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
+      <c r="H7" s="28">
+        <v>0</v>
+      </c>
+      <c r="I7" s="28">
         <v>0.60925871512226104</v>
       </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0</v>
-      </c>
-      <c r="L7" s="9">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
-        <v>0</v>
-      </c>
-      <c r="N7" s="9">
-        <v>0</v>
-      </c>
-      <c r="O7" s="9">
-        <v>0</v>
-      </c>
-      <c r="P7" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="9">
+      <c r="J7" s="28">
+        <v>0</v>
+      </c>
+      <c r="K7" s="28">
+        <v>0</v>
+      </c>
+      <c r="L7" s="29">
+        <v>0</v>
+      </c>
+      <c r="M7" s="28">
+        <v>0</v>
+      </c>
+      <c r="N7" s="29">
+        <v>0</v>
+      </c>
+      <c r="O7" s="29">
+        <v>0</v>
+      </c>
+      <c r="P7" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="29">
         <v>0</v>
       </c>
       <c r="R7" s="30">
@@ -1027,57 +1182,60 @@
       <c r="S7" s="30">
         <v>0</v>
       </c>
+      <c r="T7" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="28">
         <v>4.8471679096883651E-2</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="28">
         <v>0.34217404608508695</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="28">
         <v>0.57881671364288956</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="28">
         <v>0.11070118076464382</v>
       </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="9">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="9">
-        <v>0</v>
-      </c>
-      <c r="O8" s="9">
+      <c r="H8" s="28">
+        <v>0</v>
+      </c>
+      <c r="I8" s="28">
+        <v>0</v>
+      </c>
+      <c r="J8" s="28">
+        <v>0</v>
+      </c>
+      <c r="K8" s="28">
+        <v>0</v>
+      </c>
+      <c r="L8" s="29">
+        <v>0</v>
+      </c>
+      <c r="M8" s="28">
+        <v>0</v>
+      </c>
+      <c r="N8" s="29">
+        <v>0</v>
+      </c>
+      <c r="O8" s="29">
         <v>0.89</v>
       </c>
-      <c r="P8" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="9">
+      <c r="P8" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="29">
         <v>0</v>
       </c>
       <c r="R8" s="30">
@@ -1086,57 +1244,60 @@
       <c r="S8" s="30">
         <v>0</v>
       </c>
+      <c r="T8" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="28">
         <v>0.12956706785549071</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="28">
         <v>0.62631197989586607</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="28">
         <v>2.6859101242267806E-2</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="28">
         <v>3.4639706546678806</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="28">
         <v>0.3084245115335289</v>
       </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8">
+      <c r="I9" s="28">
+        <v>0</v>
+      </c>
+      <c r="J9" s="28">
         <v>0.84392968119641909</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="28">
         <v>0.19618427256119822</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="29">
         <v>0.74361220728073996</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="28">
         <v>0.70446163041943011</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="29">
         <v>0.66</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="29">
         <v>1.7</v>
       </c>
-      <c r="P9" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="9">
+      <c r="P9" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="29">
         <v>0.54</v>
       </c>
       <c r="R9" s="30">
@@ -1145,57 +1306,60 @@
       <c r="S9" s="30">
         <v>0</v>
       </c>
+      <c r="T9" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="28">
         <v>0.32840091228592327</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="28">
         <v>2.9950554720403061E-2</v>
       </c>
-      <c r="F10" s="8">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="28">
         <v>9.454193183755781E-2</v>
       </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="8">
-        <v>0</v>
-      </c>
-      <c r="L10" s="9">
-        <v>0</v>
-      </c>
-      <c r="M10" s="8">
-        <v>0</v>
-      </c>
-      <c r="N10" s="9">
-        <v>0</v>
-      </c>
-      <c r="O10" s="9">
-        <v>0</v>
-      </c>
-      <c r="P10" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="9">
+      <c r="H10" s="28">
+        <v>0</v>
+      </c>
+      <c r="I10" s="28">
+        <v>0</v>
+      </c>
+      <c r="J10" s="28">
+        <v>0</v>
+      </c>
+      <c r="K10" s="28">
+        <v>0</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0</v>
+      </c>
+      <c r="M10" s="28">
+        <v>0</v>
+      </c>
+      <c r="N10" s="29">
+        <v>0</v>
+      </c>
+      <c r="O10" s="29">
+        <v>0</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="29">
         <v>0</v>
       </c>
       <c r="R10" s="30">
@@ -1204,57 +1368,60 @@
       <c r="S10" s="30">
         <v>0</v>
       </c>
+      <c r="T10" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11" s="8">
-        <v>0</v>
-      </c>
-      <c r="N11" s="9">
-        <v>0</v>
-      </c>
-      <c r="O11" s="9">
-        <v>0</v>
-      </c>
-      <c r="P11" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="9">
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0</v>
+      </c>
+      <c r="H11" s="28">
+        <v>0</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0</v>
+      </c>
+      <c r="J11" s="28">
+        <v>0</v>
+      </c>
+      <c r="K11" s="28">
+        <v>0</v>
+      </c>
+      <c r="L11" s="29">
+        <v>0</v>
+      </c>
+      <c r="M11" s="28">
+        <v>0</v>
+      </c>
+      <c r="N11" s="29">
+        <v>0</v>
+      </c>
+      <c r="O11" s="29">
+        <v>0</v>
+      </c>
+      <c r="P11" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="29">
         <v>0</v>
       </c>
       <c r="R11" s="30">
@@ -1263,57 +1430,60 @@
       <c r="S11" s="30">
         <v>0</v>
       </c>
+      <c r="T11" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
         <v>1.350154710467985</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="28">
         <v>0.15903150585792669</v>
       </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+      <c r="I12" s="28">
         <v>1.0929978358411909</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="28">
         <v>0.35878879049617801</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="28">
         <v>0.41763032466165734</v>
       </c>
-      <c r="L12" s="9">
-        <v>0</v>
-      </c>
-      <c r="M12" s="8">
+      <c r="L12" s="29">
+        <v>0</v>
+      </c>
+      <c r="M12" s="28">
         <v>1.0097462857123731</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="29">
         <v>1.27</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="29">
         <v>0.32</v>
       </c>
-      <c r="P12" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="9">
+      <c r="P12" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="29">
         <v>0</v>
       </c>
       <c r="R12" s="30">
@@ -1322,57 +1492,60 @@
       <c r="S12" s="30">
         <v>0</v>
       </c>
+      <c r="T12" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:20">
+      <c r="A13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="D13" s="28">
+        <v>0</v>
+      </c>
+      <c r="E13" s="28">
         <v>2.0003135886345384E-2</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="28">
         <v>0.27039700349540563</v>
       </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8">
+      <c r="G13" s="28">
+        <v>0</v>
+      </c>
+      <c r="H13" s="28">
+        <v>0</v>
+      </c>
+      <c r="I13" s="28">
         <v>3.3045592528299583E-2</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="28">
         <v>1.546230230418145</v>
       </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="9">
-        <v>0</v>
-      </c>
-      <c r="M13" s="8">
-        <v>0</v>
-      </c>
-      <c r="N13" s="9">
-        <v>0</v>
-      </c>
-      <c r="O13" s="9">
+      <c r="K13" s="28">
+        <v>0</v>
+      </c>
+      <c r="L13" s="29">
+        <v>0</v>
+      </c>
+      <c r="M13" s="28">
+        <v>0</v>
+      </c>
+      <c r="N13" s="29">
+        <v>0</v>
+      </c>
+      <c r="O13" s="29">
         <v>0.33</v>
       </c>
-      <c r="P13" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="9">
+      <c r="P13" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="29">
         <v>0</v>
       </c>
       <c r="R13" s="30">
@@ -1381,58 +1554,105 @@
       <c r="S13" s="30">
         <v>0</v>
       </c>
+      <c r="T13" s="30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10">
-        <v>0</v>
-      </c>
-      <c r="J14" s="10">
-        <v>0</v>
-      </c>
-      <c r="K14" s="10">
-        <v>0</v>
-      </c>
-      <c r="L14" s="11">
-        <v>0</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0</v>
-      </c>
-      <c r="N14" s="10">
-        <v>0</v>
-      </c>
-      <c r="O14" s="10">
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>0</v>
-      </c>
-      <c r="R14" s="10">
+      <c r="D14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0</v>
+      </c>
+      <c r="J14" s="31">
+        <v>0</v>
+      </c>
+      <c r="K14" s="31">
+        <v>0</v>
+      </c>
+      <c r="L14" s="32">
+        <v>0</v>
+      </c>
+      <c r="M14" s="31">
+        <v>0</v>
+      </c>
+      <c r="N14" s="31">
+        <v>0</v>
+      </c>
+      <c r="O14" s="31">
+        <v>0</v>
+      </c>
+      <c r="P14" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="31">
+        <v>0</v>
+      </c>
+      <c r="R14" s="31">
         <v>1.4177257229737372</v>
       </c>
-      <c r="S14" s="10">
-        <v>0</v>
-      </c>
+      <c r="S14" s="31">
+        <v>0</v>
+      </c>
+      <c r="T14" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="34.5" customHeight="1">
+      <c r="A15" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="S4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>